<commit_message>
added : modality link color on hover for variable table and info
</commit_message>
<xml_diff>
--- a/data/db_source/evolution.xlsx
+++ b/data/db_source/evolution.xlsx
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>2011</t>
+  </si>
+  <si>
+    <t>dep_sante___variable_3</t>
   </si>
 </sst>
 </file>
@@ -394,6 +397,29 @@
         <v>11</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9">
+        <v>1746359037</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>